<commit_message>
Added offline mode to event audio files.
</commit_message>
<xml_diff>
--- a/data/AVAnnotate Event Template.xlsx
+++ b/data/AVAnnotate Event Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorinjameson/Work/AVAnnotate/admin-client/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3905504-020D-4840-9370-D40815CF85B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D926B72-10F9-DE46-A301-4617591A2310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="3520" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30600" yWindow="3380" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Event Label</t>
   </si>
@@ -35,67 +35,21 @@
     <t>Event Citation (optional)</t>
   </si>
   <si>
-    <t>Interview 1</t>
-  </si>
-  <si>
-    <t>Audio</t>
-  </si>
-  <si>
-    <t>url1</t>
-  </si>
-  <si>
-    <t>Interview 2</t>
-  </si>
-  <si>
-    <t>url2</t>
-  </si>
-  <si>
     <t>AVFile Label (might be the same as event label)</t>
   </si>
   <si>
-    <t>Tape 1</t>
-  </si>
-  <si>
-    <t>Tape 2</t>
-  </si>
-  <si>
-    <t>Tape 3</t>
-  </si>
-  <si>
-    <t>url3</t>
-  </si>
-  <si>
     <t>Event Description (Optional)</t>
-  </si>
-  <si>
-    <t>Just plain text</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;Bold&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>&lt;em&gt;Italics&lt;/em&gt;</t>
-  </si>
-  <si>
-    <t>Interview 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -135,11 +89,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,10 +311,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -372,75 +325,24 @@
     <col min="6" max="6" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>